<commit_message>
Finished Progression Chart file
Has shiny graph-y bits now also alot of data.
</commit_message>
<xml_diff>
--- a/Documentation/Progression Chart.xlsx
+++ b/Documentation/Progression Chart.xlsx
@@ -15,8 +15,234 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Kent Frauendienst</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These are not additive - it's the time difference from the point at which it evolved into this form.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is the rate at which checks are run after the initial evolution check, to check again and see if it'll evolve.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The amount of progression points required to trigger evolution when an evolution check happens.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The lowest possible amount the player can lower the progression point requirement to through whatever means.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The progression point requirement cap.  It cannot increase past this point.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Every hour, the required number of progression points increases by this amount, up to the cap.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+How many progression points are granted to the monster during this stage of evolution when a text message is sent or received.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Assuming someone gets the required amount of progression points to trigger evolution at the initial point in every stage, this is how long it will take to evolve past this point.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Kent Frauendienst:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+How many text messages you'll need to send in this stage to reach the initial progression point requirement for evolution.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Egg</t>
   </si>
@@ -77,21 +303,56 @@
   <si>
     <t>Initial PPR (progression points required for evolution)</t>
   </si>
+  <si>
+    <t>Total Minimum Time</t>
+  </si>
+  <si>
+    <t>SMS Required for Initial PPR</t>
+  </si>
+  <si>
+    <t>SMS Required for Minimum PPR</t>
+  </si>
+  <si>
+    <t>SMS Required for Maximum PPR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
-  </numFmts>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,10 +375,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,6 +385,1099 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Progression Point</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Growth Curve</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.7856345873843574E-2"/>
+          <c:y val="0.23089194142702968"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33827538623540332"/>
+          <c:y val="3.1748695104212396E-2"/>
+          <c:w val="0.66172461376459712"/>
+          <c:h val="0.70539345711759516"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Initial PPR (progression points required for evolution)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Egg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baby 0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baby 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Baby 2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Baby 3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Adolescent 0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adolescent 1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Adolescent 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Adolescent 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Adult 0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Adult 1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Adult 2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Adult 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1920</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Minimum PPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Egg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baby 0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baby 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Baby 2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Baby 3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Adolescent 0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adolescent 1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Adolescent 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Adolescent 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Adult 0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Adult 1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Adult 2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Adult 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Maximum PPR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Egg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baby 0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baby 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Baby 2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Baby 3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Adolescent 0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adolescent 1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Adolescent 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Adolescent 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Adult 0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Adult 1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Adult 2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Adult 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2560</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="127756928"/>
+        <c:axId val="127775104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="127756928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="127775104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="127775104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Progression</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Points Required for Evolution</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.27710848050617293"/>
+              <c:y val="0.10851479331506922"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="127756928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time until Initial Evolution Check</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Egg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baby 0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baby 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Baby 2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Baby 3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Adolescent 0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adolescent 1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Adolescent 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Adolescent 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Adult 0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Adult 1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Adult 2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Adult 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>[h]:mm:ss</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.3888888888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.472222222222222E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0833333333333332E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="127940096"/>
+        <c:axId val="127941632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="127940096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[h]:mm:ss;@" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="127941632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="127941632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[h]:mm:ss" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="127940096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Minimum Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Egg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baby 0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baby 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Baby 2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Baby 3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Adolescent 0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adolescent 1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Adolescent 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Adolescent 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Adult 0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Adult 1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Adult 2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Adult 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>[h]:mm:ss</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.3888888888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8611111111111112E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5694444444444443E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10902777777777778</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35902777777777778</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85902777777777772</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6090277777777777</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1090277777777775</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1090277777777775</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.4423611111111114</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.442361111111111</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.442361111111111</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25.442361111111111</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="127986304"/>
+        <c:axId val="127992192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="127986304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="127992192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="127992192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[h]:mm:ss" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="127986304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.6475833333333334"/>
+          <c:y val="0.18725029163021295"/>
+          <c:w val="0.19408333333333336"/>
+          <c:h val="0.22723571011956839"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Subsequent Evolution Check Interval</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Egg</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Baby 0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Baby 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Baby 2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Baby 3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Adolescent 0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Adolescent 1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Adolescent 2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Adolescent 3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Adult 0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Adult 1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Adult 2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Adult 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>[h]:mm:ss</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1.3888888888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.472222222222222E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9444444444444441E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.125E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3333333333333329E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15972222222222224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.20833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.41666666666666669</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="52345856"/>
+        <c:axId val="52349184"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="52345856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="52349184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="52349184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="[h]:mm:ss" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="52345856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228601</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>704849</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,10 +1765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -426,6 +1779,7 @@
     <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -473,57 +1827,44 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2">
-        <f>TIME(0,2,0)</f>
+      <c r="B2" s="1">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="C2" s="1">
-        <f>TIME(0,5,0)</f>
         <v>3.472222222222222E-3</v>
       </c>
       <c r="D2" s="1">
-        <f>TIME(0,30,0)</f>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E2" s="1">
-        <f>TIME(2,0,0)</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F2" s="1">
-        <f>TIME(6,0,0)</f>
         <v>0.25</v>
       </c>
       <c r="G2" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.75</v>
       </c>
       <c r="I2" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>1.5</v>
       </c>
       <c r="J2" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>3</v>
       </c>
       <c r="K2" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="L2" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>5</v>
       </c>
       <c r="N2" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -531,56 +1872,43 @@
         <v>16</v>
       </c>
       <c r="B3" s="1">
-        <f>TIME(0,2,0)</f>
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="C3" s="1">
-        <f>TIME(0,5,0)</f>
         <v>3.472222222222222E-3</v>
       </c>
       <c r="D3" s="1">
-        <f>TIME(0,10,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="E3" s="1">
-        <f>TIME(0,45,0)</f>
         <v>3.125E-2</v>
       </c>
       <c r="F3" s="1">
-        <f>TIME(2,0,0)</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="G3" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.125</v>
       </c>
       <c r="H3" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.15972222222222224</v>
       </c>
       <c r="I3" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.1875</v>
       </c>
       <c r="J3" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="K3" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.25</v>
       </c>
       <c r="L3" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.3125</v>
       </c>
       <c r="M3" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="N3" s="1">
-        <f>TIME(0,2,0)</f>
-        <v>1.3888888888888889E-3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -602,6 +1930,30 @@
       <c r="F4">
         <v>200</v>
       </c>
+      <c r="G4">
+        <v>640</v>
+      </c>
+      <c r="H4">
+        <v>720</v>
+      </c>
+      <c r="I4">
+        <v>900</v>
+      </c>
+      <c r="J4">
+        <v>1280</v>
+      </c>
+      <c r="K4">
+        <v>1440</v>
+      </c>
+      <c r="L4">
+        <v>1920</v>
+      </c>
+      <c r="M4">
+        <v>2560</v>
+      </c>
+      <c r="N4">
+        <v>3200</v>
+      </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
@@ -611,16 +1963,52 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <f>QUOTIENT(C4,2)</f>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <f>QUOTIENT(D4,2)</f>
+        <v>25</v>
       </c>
       <c r="E5">
+        <f>QUOTIENT(E4,2)</f>
         <v>50</v>
       </c>
       <c r="F5">
+        <f>QUOTIENT(F4,2)</f>
         <v>100</v>
+      </c>
+      <c r="G5">
+        <f>QUOTIENT(G4,2)</f>
+        <v>320</v>
+      </c>
+      <c r="H5">
+        <f>QUOTIENT(H4,2)</f>
+        <v>360</v>
+      </c>
+      <c r="I5">
+        <f>QUOTIENT(I4,2)</f>
+        <v>450</v>
+      </c>
+      <c r="J5">
+        <f>QUOTIENT(J4,2)</f>
+        <v>640</v>
+      </c>
+      <c r="K5">
+        <f>QUOTIENT(K4,2)</f>
+        <v>720</v>
+      </c>
+      <c r="L5">
+        <f>QUOTIENT(L4,2)</f>
+        <v>960</v>
+      </c>
+      <c r="M5">
+        <f>QUOTIENT(M4,2)</f>
+        <v>1280</v>
+      </c>
+      <c r="N5">
+        <f>QUOTIENT(N4,2)</f>
+        <v>1600</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -631,16 +2019,52 @@
         <v>10</v>
       </c>
       <c r="C6">
+        <f>PRODUCT(C4,1.5)</f>
         <v>30</v>
       </c>
       <c r="D6">
+        <f>PRODUCT(D4,1.5)</f>
         <v>75</v>
       </c>
       <c r="E6">
+        <f>PRODUCT(E4,1.5)</f>
         <v>150</v>
       </c>
       <c r="F6">
+        <f>PRODUCT(F4,1.5)</f>
         <v>300</v>
+      </c>
+      <c r="G6">
+        <f>PRODUCT(G4,2)</f>
+        <v>1280</v>
+      </c>
+      <c r="H6">
+        <f>PRODUCT(H4,2)</f>
+        <v>1440</v>
+      </c>
+      <c r="I6">
+        <f>PRODUCT(I4,2)</f>
+        <v>1800</v>
+      </c>
+      <c r="J6">
+        <f>PRODUCT(J4,2)</f>
+        <v>2560</v>
+      </c>
+      <c r="K6">
+        <f>PRODUCT(K4,2.5)</f>
+        <v>3600</v>
+      </c>
+      <c r="L6">
+        <f>PRODUCT(L4,2.5)</f>
+        <v>4800</v>
+      </c>
+      <c r="M6">
+        <f>PRODUCT(M4,2.5)</f>
+        <v>6400</v>
+      </c>
+      <c r="N6">
+        <f>PRODUCT(N4,2.5)</f>
+        <v>8000</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -662,6 +2086,30 @@
       <c r="F7">
         <v>2</v>
       </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
@@ -683,33 +2131,263 @@
         <v>10</v>
       </c>
       <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>12</v>
+      </c>
+      <c r="K8">
+        <v>15</v>
+      </c>
+      <c r="L8">
+        <v>15</v>
+      </c>
+      <c r="M8">
+        <v>15</v>
+      </c>
+      <c r="N8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <f>B2</f>
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9:N9" si="0">B9+C2</f>
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5694444444444443E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.10902777777777778</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.35902777777777778</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.85902777777777772</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6090277777777777</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1090277777777775</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>6.1090277777777775</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>9.4423611111111114</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="0"/>
+        <v>13.442361111111111</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>18.442361111111111</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="0"/>
+        <v>25.442361111111111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <f>QUOTIENT(B4,B8)</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>QUOTIENT(C4,C8)</f>
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <f>QUOTIENT(D4,D8)</f>
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <f>QUOTIENT(E4,E8)</f>
         <v>10</v>
       </c>
-      <c r="H8">
+      <c r="F10">
+        <f>QUOTIENT(F4,F8)</f>
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <f>QUOTIENT(G4,G8)</f>
+        <v>53</v>
+      </c>
+      <c r="H10">
+        <f>QUOTIENT(H4,H8)</f>
+        <v>60</v>
+      </c>
+      <c r="I10">
+        <f>QUOTIENT(I4,I8)</f>
+        <v>75</v>
+      </c>
+      <c r="J10">
+        <f>QUOTIENT(J4,J8)</f>
+        <v>106</v>
+      </c>
+      <c r="K10">
+        <f>QUOTIENT(K4,K8)</f>
+        <v>96</v>
+      </c>
+      <c r="L10">
+        <f>QUOTIENT(L4,L8)</f>
+        <v>128</v>
+      </c>
+      <c r="M10">
+        <f>QUOTIENT(M4,M8)</f>
+        <v>170</v>
+      </c>
+      <c r="N10">
+        <f>QUOTIENT(N4,N8)</f>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <f>QUOTIENT(B5,B8)</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:N11" si="1">QUOTIENT(C5,C8)</f>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I8">
-        <v>10</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="K8">
-        <v>10</v>
-      </c>
-      <c r="L8">
-        <v>10</v>
-      </c>
-      <c r="M8">
-        <v>10</v>
-      </c>
-      <c r="N8">
-        <v>10</v>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <f>QUOTIENT(B6,B8)</f>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:N12" si="2">QUOTIENT(C6,C8)</f>
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>426</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>533</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>